<commit_message>
update simple model and the result of accuracy 88% without finetune
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -10,11 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="80">
   <si>
     <t>是否数据增广</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -277,6 +278,62 @@
   </si>
   <si>
     <t>验证集比例（大小）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>390s + 291s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>230s * 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1140s * 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600s * 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(250, 250, 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>204s * 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>208s * 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bbox数据进行了进一步清洗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600s * 50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -629,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -642,16 +699,17 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.109375" customWidth="1"/>
     <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -668,37 +726,43 @@
         <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -714,38 +778,41 @@
       <c r="E2" s="1">
         <v>0.2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1">
-        <v>2000</v>
-      </c>
       <c r="H2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>0.1792</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>0.91479999999999995</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>1.9117999999999999</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>0.7</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -761,38 +828,41 @@
       <c r="E3" s="1">
         <v>0.2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1">
-        <v>2000</v>
-      </c>
       <c r="H3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="1">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>0.24929999999999999</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>0.95930000000000004</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>2.7688000000000001</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>0.7</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -808,38 +878,41 @@
       <c r="E4" s="1">
         <v>0.2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1">
-        <v>2000</v>
-      </c>
       <c r="H4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1">
         <v>0.18240000000000001</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>0.90980000000000005</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>2.2441</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>0.71</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -855,38 +928,41 @@
       <c r="E5" s="1">
         <v>0.2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1">
-        <v>2000</v>
-      </c>
       <c r="H5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="1">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1">
         <v>7.9711999999999996</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>0.5</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>7.9711999999999996</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>0.5</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -902,38 +978,41 @@
       <c r="E6" s="1">
         <v>0.2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="1">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1">
-        <v>2000</v>
-      </c>
       <c r="H6" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="1">
+        <v>9</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="1">
         <v>0.52170000000000005</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>0.66259999999999997</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>2.1573000000000002</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>0.54749999999999999</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -949,38 +1028,41 @@
       <c r="E7" s="1">
         <v>0.2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="1">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1">
-        <v>2000</v>
-      </c>
       <c r="H7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="1">
+        <v>9</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1">
         <v>0.2457</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>0.89200000000000002</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>1.492</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>0.65749999999999997</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -996,38 +1078,41 @@
       <c r="E8" s="1">
         <v>0.2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="1">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>100</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>20</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="1">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1">
         <v>0.51690000000000003</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>0.75280000000000002</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>0.56359999999999999</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>0.69</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1043,38 +1128,41 @@
       <c r="E9" s="1">
         <v>0.2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="1">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="1">
-        <v>2000</v>
-      </c>
       <c r="H9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I9" s="1">
         <v>42</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="1">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1">
         <v>6.9800000000000001E-2</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>0.9758</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>0.97540000000000004</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>0.83</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1090,23 +1178,26 @@
       <c r="E10" s="1">
         <v>0.2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="1">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="1">
-        <v>2000</v>
-      </c>
       <c r="H10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I10" s="1">
         <v>50</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1122,23 +1213,26 @@
       <c r="E11" s="1">
         <v>0.2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="1">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="1">
-        <v>2000</v>
-      </c>
       <c r="H11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="1">
         <v>50</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1154,38 +1248,41 @@
       <c r="E12" s="1">
         <v>0.2</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="1">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="1">
-        <v>2000</v>
-      </c>
       <c r="H12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="1">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1">
         <v>0.24779999999999999</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>0.87070000000000003</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>1.4215</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>0.72</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1201,38 +1298,41 @@
       <c r="E13" s="1">
         <v>0.2</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="1">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="1">
-        <v>2000</v>
-      </c>
       <c r="H13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="1">
+        <v>9</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1">
         <v>0.38669999999999999</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>0.8</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>1.22</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>0.7</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1248,38 +1348,41 @@
       <c r="E14" s="1">
         <v>0.2</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="1">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="1">
-        <v>2000</v>
-      </c>
       <c r="H14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="1">
+        <v>9</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1">
         <v>0.1444</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>0.92869999999999997</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>1.6466000000000001</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>0.73</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1295,38 +1398,41 @@
       <c r="E15" s="1">
         <v>0.2</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="1">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1">
-        <v>2000</v>
-      </c>
       <c r="H15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I15" s="1">
         <v>1</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="1">
+        <v>9</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="1">
         <v>0.2112</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>0.88670000000000004</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>1.5486</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>0.71</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1342,38 +1448,41 @@
       <c r="E16" s="1">
         <v>0.2</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="1">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="1">
-        <v>2000</v>
-      </c>
       <c r="H16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I16" s="1">
         <v>2</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="1">
+        <v>9</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="1">
         <v>1.34E-2</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>0.99570000000000003</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>1.8555999999999999</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>0.72</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1389,38 +1498,41 @@
       <c r="E17" s="1">
         <v>0.2</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="1">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="1">
-        <v>2000</v>
-      </c>
       <c r="H17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I17" s="1">
         <v>2</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="1">
+        <v>9</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="1">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>0.99399999999999999</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>2.71</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O17" s="1">
         <v>0.7</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1436,38 +1548,41 @@
       <c r="E18" s="1">
         <v>0.2</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="1">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="1">
-        <v>2000</v>
-      </c>
       <c r="H18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I18" s="1">
         <v>2</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="1">
+        <v>9</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="1">
         <v>2.53E-2</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>0.98880000000000001</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>2.3445</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>0.68</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1483,38 +1598,41 @@
       <c r="E19" s="1">
         <v>0.2</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="1">
+        <v>32</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="1">
-        <v>2000</v>
-      </c>
       <c r="H19" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I19" s="1">
         <v>2</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="1">
+        <v>9</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="1">
         <v>1.55E-2</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>0.99509999999999998</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>2.4542000000000002</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O19" s="1">
         <v>0.68500000000000005</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1530,38 +1648,41 @@
       <c r="E20" s="1">
         <v>0.2</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="1">
+        <v>32</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="1">
-        <v>2000</v>
-      </c>
       <c r="H20" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I20" s="1">
         <v>2</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="1">
+        <v>9</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="L20" s="1">
+      <c r="M20" s="1">
         <v>0.99929999999999997</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <v>3.3294999999999999</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>0.66500000000000004</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1577,38 +1698,41 @@
       <c r="E21" s="1">
         <v>0.2</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="1">
+        <v>32</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="1">
-        <v>2000</v>
-      </c>
       <c r="H21" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I21" s="1">
         <v>2</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="1">
+        <v>9</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="1">
         <v>0.13020000000000001</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>0.93569999999999998</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>4.1432000000000002</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>0.54749999999999999</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1624,38 +1748,41 @@
       <c r="E22" s="1">
         <v>0.2</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="1">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="1">
-        <v>2000</v>
-      </c>
       <c r="H22" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="1">
         <v>3</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="1">
+        <v>9</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="1">
         <v>6.6500000000000004E-2</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>0.97570000000000001</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>1.2710999999999999</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>0.73</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1671,38 +1798,41 @@
       <c r="E23" s="1">
         <v>0.2</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="1">
+        <v>32</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="1">
-        <v>2000</v>
-      </c>
       <c r="H23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I23" s="1">
         <v>2</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K23" s="1">
+        <v>9</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="1">
         <v>2.7099999999999999E-2</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>0.99139999999999995</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>2.0712999999999999</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>0.63</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1718,38 +1848,41 @@
       <c r="E24" s="1">
         <v>0.2</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="1">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="1">
-        <v>2000</v>
-      </c>
       <c r="H24" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I24" s="1">
         <v>50</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" s="1">
+        <v>9</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="1">
         <v>9.1499999999999998E-2</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>0.96609999999999996</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>1.2065999999999999</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>0.76</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1765,38 +1898,41 @@
       <c r="E25" s="1">
         <v>0.2</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="1">
+        <v>32</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="1">
-        <v>2000</v>
-      </c>
       <c r="H25" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I25" s="1">
         <v>20</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="1">
+        <v>9</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="1">
         <v>0.13519999999999999</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <v>0.95030000000000003</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <v>0.62839999999999996</v>
       </c>
-      <c r="N25" s="1">
+      <c r="O25" s="1">
         <v>0.83</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1812,38 +1948,41 @@
       <c r="E26" s="1">
         <v>0.2</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="1">
+        <v>32</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="1">
-        <v>2000</v>
-      </c>
       <c r="H26" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I26" s="1">
         <v>50</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="1">
+        <v>9</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="1">
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <v>0.97670000000000001</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <v>1.0512999999999999</v>
       </c>
-      <c r="N26" s="1">
+      <c r="O26" s="1">
         <v>0.77</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1859,38 +1998,41 @@
       <c r="E27" s="1">
         <v>0.2</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="1">
+        <v>32</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="1">
-        <v>2000</v>
-      </c>
       <c r="H27" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I27" s="1">
         <v>23</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="1">
+        <v>9</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="1">
         <v>4.87E-2</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <v>0.98319999999999996</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <v>0.96050000000000002</v>
       </c>
-      <c r="N27" s="1">
+      <c r="O27" s="1">
         <v>0.83</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1906,38 +2048,41 @@
       <c r="E28" s="1">
         <v>0.2</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="1">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="1">
-        <v>2000</v>
-      </c>
       <c r="H28" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I28" s="1">
         <v>2</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K28" s="1">
+        <v>9</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="1">
         <v>1.12E-2</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <v>0.99639999999999995</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <v>2.0585</v>
       </c>
-      <c r="N28" s="1">
+      <c r="O28" s="1">
         <v>0.71</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1953,35 +2098,391 @@
       <c r="E29" s="1">
         <v>23000</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="1">
+        <v>32</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="1">
-        <v>2000</v>
-      </c>
       <c r="H29" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I29" s="1">
         <v>2</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>1.47E-2</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <v>0.99550000000000005</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <v>2.3279000000000001</v>
       </c>
-      <c r="N29" s="1">
+      <c r="O29" s="1">
         <v>0.68530000000000002</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F30" s="1">
+        <v>32</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="N30" s="1">
+        <v>3.1293000000000002</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F31" s="1">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I31" s="1">
+        <v>5</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" s="1">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1.3498000000000001</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0.73780000000000001</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F32" s="1">
+        <v>32</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1.84E-2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2.0674000000000001</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0.63490000000000002</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F33" s="1">
+        <v>32</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I33" s="1">
+        <v>20</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.17330000000000001</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0.93279999999999996</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0.87029999999999996</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0.8165</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F34" s="1">
+        <v>32</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I34" s="1">
+        <v>50</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0.1069</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0.9607</v>
+      </c>
+      <c r="N34" s="1">
+        <v>1.0205</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0.78549999999999998</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F35" s="1">
+        <v>32</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I35" s="1">
+        <v>50</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="1">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0.9788</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0.98119999999999996</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="1">
+        <v>23000</v>
+      </c>
+      <c r="F36" s="1">
+        <v>16</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I36" s="1">
+        <v>50</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L36" s="1">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0.98240000000000005</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0.48659999999999998</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0.88490000000000002</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do some expriments and no progress
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -1,371 +1,575 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView windowWidth="20490" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
+  <si>
+    <t>是否有bbox</t>
+  </si>
   <si>
     <t>是否数据增广</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像大小</t>
   </si>
   <si>
     <t>模型选择</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证集比例（大小）</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>最后一层激活函数</t>
   </si>
   <si>
     <t>step_per_epoch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>epochs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>loss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>optimizer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <t>val_loss</t>
   </si>
   <si>
     <t>val_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所用时间</t>
+  </si>
+  <si>
+    <t>备注</t>
   </si>
   <si>
     <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(150, 150, 3)</t>
+  </si>
+  <si>
+    <t>三层卷积池化后激活</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>binary_crossentropy</t>
   </si>
   <si>
     <t>rmsprop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>binary_crossentropy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>所用时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>180s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最后一层激活函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sigmoid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>180s * 10</t>
   </si>
   <si>
     <t>adam</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>180s * 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>167s</t>
   </si>
   <si>
     <t>softmax</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>loss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>val_loss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>167s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>167s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AlexNet_model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sigmoid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>184s</t>
   </si>
   <si>
     <t>dnn_model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>184s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>232s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图像大小</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(150, 150, 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>24s * 20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否有bbox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>490s * 42</t>
   </si>
   <si>
     <t>(50, 50, 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>154s</t>
   </si>
   <si>
     <t>(100, 100, 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>151s</t>
   </si>
   <si>
     <t>(200, 200, 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>182s</t>
   </si>
   <si>
     <t>(250, 250, 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>490s * 42</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>154s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>151s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>182s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>198s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>140s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>157s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>180s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>198s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>150s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三层卷积池化后激活</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>340s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>146s * 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>535s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>183s * 50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1050s * 20</t>
   </si>
   <si>
     <t>200s * 50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1050s * 20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1078s * 23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>180s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adam</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>326s + 234s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>验证集比例（大小）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>390s + 291s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>230s * 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600s * 2</t>
   </si>
   <si>
     <t>1140s * 20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>600s * 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(250, 250, 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>204s * 50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>208s * 50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600s * 50</t>
   </si>
   <si>
     <t>bbox数据进行了进一步清洗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>600s * 50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -373,9 +577,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -383,17 +829,61 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -442,7 +932,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,7 +967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -680,100 +1170,100 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.5583333333333" customWidth="1"/>
+    <col min="2" max="2" width="13.775" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="20.3333333333333" customWidth="1"/>
+    <col min="6" max="6" width="12.8833333333333" customWidth="1"/>
+    <col min="7" max="7" width="17.775" customWidth="1"/>
+    <col min="8" max="8" width="17.4416666666667" customWidth="1"/>
+    <col min="9" max="9" width="10.5583333333333" customWidth="1"/>
+    <col min="10" max="10" width="27.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="12.1083333333333" customWidth="1"/>
+    <col min="15" max="15" width="11.6666666666667" customWidth="1"/>
+    <col min="16" max="16" width="12.4416666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="1">
         <v>0.2</v>
@@ -782,7 +1272,7 @@
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1">
         <v>2000</v>
@@ -791,39 +1281,39 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="L2" s="1">
         <v>0.1792</v>
       </c>
       <c r="M2" s="1">
-        <v>0.91479999999999995</v>
+        <v>0.9148</v>
       </c>
       <c r="N2" s="1">
-        <v>1.9117999999999999</v>
+        <v>1.9118</v>
       </c>
       <c r="O2" s="1">
         <v>0.7</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1">
         <v>0.2</v>
@@ -832,7 +1322,7 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1">
         <v>2000</v>
@@ -841,39 +1331,39 @@
         <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="L3" s="1">
-        <v>0.24929999999999999</v>
+        <v>0.2493</v>
       </c>
       <c r="M3" s="1">
-        <v>0.95930000000000004</v>
+        <v>0.9593</v>
       </c>
       <c r="N3" s="1">
-        <v>2.7688000000000001</v>
+        <v>2.7688</v>
       </c>
       <c r="O3" s="1">
         <v>0.7</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>0.2</v>
@@ -882,7 +1372,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1">
         <v>2000</v>
@@ -891,16 +1381,16 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L4" s="1">
-        <v>0.18240000000000001</v>
+        <v>0.1824</v>
       </c>
       <c r="M4" s="1">
-        <v>0.90980000000000005</v>
+        <v>0.9098</v>
       </c>
       <c r="N4" s="1">
         <v>2.2441</v>
@@ -909,21 +1399,21 @@
         <v>0.71</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1">
         <v>0.2</v>
@@ -932,7 +1422,7 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1">
         <v>2000</v>
@@ -941,39 +1431,39 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L5" s="1">
-        <v>7.9711999999999996</v>
+        <v>7.9712</v>
       </c>
       <c r="M5" s="1">
         <v>0.5</v>
       </c>
       <c r="N5" s="1">
-        <v>7.9711999999999996</v>
+        <v>7.9712</v>
       </c>
       <c r="O5" s="1">
         <v>0.5</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
         <v>0.2</v>
@@ -982,7 +1472,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H6" s="1">
         <v>2000</v>
@@ -991,39 +1481,39 @@
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L6" s="1">
-        <v>0.52170000000000005</v>
+        <v>0.5217</v>
       </c>
       <c r="M6" s="1">
-        <v>0.66259999999999997</v>
+        <v>0.6626</v>
       </c>
       <c r="N6" s="1">
-        <v>2.1573000000000002</v>
+        <v>2.1573</v>
       </c>
       <c r="O6" s="1">
-        <v>0.54749999999999999</v>
+        <v>0.5475</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1">
         <v>0.2</v>
@@ -1032,7 +1522,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1">
         <v>2000</v>
@@ -1041,39 +1531,39 @@
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L7" s="1">
         <v>0.2457</v>
       </c>
       <c r="M7" s="1">
-        <v>0.89200000000000002</v>
+        <v>0.892</v>
       </c>
       <c r="N7" s="1">
         <v>1.492</v>
       </c>
       <c r="O7" s="1">
-        <v>0.65749999999999997</v>
+        <v>0.6575</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1">
         <v>0.2</v>
@@ -1082,7 +1572,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1">
         <v>100</v>
@@ -1091,39 +1581,39 @@
         <v>20</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L8" s="1">
-        <v>0.51690000000000003</v>
+        <v>0.5169</v>
       </c>
       <c r="M8" s="1">
-        <v>0.75280000000000002</v>
+        <v>0.7528</v>
       </c>
       <c r="N8" s="1">
-        <v>0.56359999999999999</v>
+        <v>0.5636</v>
       </c>
       <c r="O8" s="1">
         <v>0.69</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1">
         <v>0.2</v>
@@ -1132,7 +1622,7 @@
         <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H9" s="1">
         <v>2000</v>
@@ -1141,39 +1631,39 @@
         <v>42</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L9" s="1">
-        <v>6.9800000000000001E-2</v>
+        <v>0.0698</v>
       </c>
       <c r="M9" s="1">
         <v>0.9758</v>
       </c>
       <c r="N9" s="1">
-        <v>0.97540000000000004</v>
+        <v>0.9754</v>
       </c>
       <c r="O9" s="1">
         <v>0.83</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1">
         <v>0.2</v>
@@ -1182,7 +1672,7 @@
         <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H10" s="1">
         <v>2000</v>
@@ -1191,24 +1681,24 @@
         <v>50</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E11" s="1">
         <v>0.2</v>
@@ -1217,7 +1707,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H11" s="1">
         <v>2000</v>
@@ -1226,24 +1716,24 @@
         <v>50</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1">
         <v>0.2</v>
@@ -1252,7 +1742,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1">
         <v>2000</v>
@@ -1261,16 +1751,16 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L12" s="1">
-        <v>0.24779999999999999</v>
+        <v>0.2478</v>
       </c>
       <c r="M12" s="1">
-        <v>0.87070000000000003</v>
+        <v>0.8707</v>
       </c>
       <c r="N12" s="1">
         <v>1.4215</v>
@@ -1279,21 +1769,21 @@
         <v>0.72</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1">
         <v>0.2</v>
@@ -1302,7 +1792,7 @@
         <v>32</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H13" s="1">
         <v>2000</v>
@@ -1311,13 +1801,13 @@
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L13" s="1">
-        <v>0.38669999999999999</v>
+        <v>0.3867</v>
       </c>
       <c r="M13" s="1">
         <v>0.8</v>
@@ -1329,21 +1819,21 @@
         <v>0.7</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E14" s="1">
         <v>0.2</v>
@@ -1352,7 +1842,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H14" s="1">
         <v>2000</v>
@@ -1361,39 +1851,39 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L14" s="1">
         <v>0.1444</v>
       </c>
       <c r="M14" s="1">
-        <v>0.92869999999999997</v>
+        <v>0.9287</v>
       </c>
       <c r="N14" s="1">
-        <v>1.6466000000000001</v>
+        <v>1.6466</v>
       </c>
       <c r="O14" s="1">
         <v>0.73</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E15" s="1">
         <v>0.2</v>
@@ -1402,7 +1892,7 @@
         <v>32</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H15" s="1">
         <v>2000</v>
@@ -1411,16 +1901,16 @@
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L15" s="1">
         <v>0.2112</v>
       </c>
       <c r="M15" s="1">
-        <v>0.88670000000000004</v>
+        <v>0.8867</v>
       </c>
       <c r="N15" s="1">
         <v>1.5486</v>
@@ -1429,21 +1919,21 @@
         <v>0.71</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E16" s="1">
         <v>0.2</v>
@@ -1452,7 +1942,7 @@
         <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H16" s="1">
         <v>2000</v>
@@ -1461,39 +1951,39 @@
         <v>2</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L16" s="1">
-        <v>1.34E-2</v>
+        <v>0.0134</v>
       </c>
       <c r="M16" s="1">
-        <v>0.99570000000000003</v>
+        <v>0.9957</v>
       </c>
       <c r="N16" s="1">
-        <v>1.8555999999999999</v>
+        <v>1.8556</v>
       </c>
       <c r="O16" s="1">
         <v>0.72</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1">
         <v>0.2</v>
@@ -1502,7 +1992,7 @@
         <v>32</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H17" s="1">
         <v>2000</v>
@@ -1511,16 +2001,16 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L17" s="1">
-        <v>1.2699999999999999E-2</v>
+        <v>0.0127</v>
       </c>
       <c r="M17" s="1">
-        <v>0.99399999999999999</v>
+        <v>0.994</v>
       </c>
       <c r="N17" s="1">
         <v>2.71</v>
@@ -1529,21 +2019,21 @@
         <v>0.7</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E18" s="1">
         <v>0.2</v>
@@ -1552,7 +2042,7 @@
         <v>32</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H18" s="1">
         <v>2000</v>
@@ -1561,16 +2051,16 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L18" s="1">
-        <v>2.53E-2</v>
+        <v>0.0253</v>
       </c>
       <c r="M18" s="1">
-        <v>0.98880000000000001</v>
+        <v>0.9888</v>
       </c>
       <c r="N18" s="1">
         <v>2.3445</v>
@@ -1579,21 +2069,21 @@
         <v>0.68</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1">
         <v>0.2</v>
@@ -1602,7 +2092,7 @@
         <v>32</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H19" s="1">
         <v>2000</v>
@@ -1611,39 +2101,39 @@
         <v>2</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L19" s="1">
-        <v>1.55E-2</v>
+        <v>0.0155</v>
       </c>
       <c r="M19" s="1">
-        <v>0.99509999999999998</v>
+        <v>0.9951</v>
       </c>
       <c r="N19" s="1">
-        <v>2.4542000000000002</v>
+        <v>2.4542</v>
       </c>
       <c r="O19" s="1">
-        <v>0.68500000000000005</v>
+        <v>0.685</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1">
         <v>0.2</v>
@@ -1652,7 +2142,7 @@
         <v>32</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H20" s="1">
         <v>2000</v>
@@ -1661,39 +2151,39 @@
         <v>2</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L20" s="1">
-        <v>2.2000000000000001E-3</v>
+        <v>0.0022</v>
       </c>
       <c r="M20" s="1">
-        <v>0.99929999999999997</v>
+        <v>0.9993</v>
       </c>
       <c r="N20" s="1">
-        <v>3.3294999999999999</v>
+        <v>3.3295</v>
       </c>
       <c r="O20" s="1">
-        <v>0.66500000000000004</v>
+        <v>0.665</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E21" s="1">
         <v>0.2</v>
@@ -1702,7 +2192,7 @@
         <v>32</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H21" s="1">
         <v>2000</v>
@@ -1711,39 +2201,39 @@
         <v>2</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L21" s="1">
-        <v>0.13020000000000001</v>
+        <v>0.1302</v>
       </c>
       <c r="M21" s="1">
-        <v>0.93569999999999998</v>
+        <v>0.9357</v>
       </c>
       <c r="N21" s="1">
-        <v>4.1432000000000002</v>
+        <v>4.1432</v>
       </c>
       <c r="O21" s="1">
-        <v>0.54749999999999999</v>
+        <v>0.5475</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E22" s="1">
         <v>0.2</v>
@@ -1752,7 +2242,7 @@
         <v>32</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H22" s="1">
         <v>2000</v>
@@ -1761,39 +2251,39 @@
         <v>3</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L22" s="1">
-        <v>6.6500000000000004E-2</v>
+        <v>0.0665</v>
       </c>
       <c r="M22" s="1">
-        <v>0.97570000000000001</v>
+        <v>0.9757</v>
       </c>
       <c r="N22" s="1">
-        <v>1.2710999999999999</v>
+        <v>1.2711</v>
       </c>
       <c r="O22" s="1">
         <v>0.73</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1">
         <v>0.2</v>
@@ -1802,7 +2292,7 @@
         <v>32</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H23" s="1">
         <v>2000</v>
@@ -1811,39 +2301,39 @@
         <v>2</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L23" s="1">
-        <v>2.7099999999999999E-2</v>
+        <v>0.0271</v>
       </c>
       <c r="M23" s="1">
-        <v>0.99139999999999995</v>
+        <v>0.9914</v>
       </c>
       <c r="N23" s="1">
-        <v>2.0712999999999999</v>
+        <v>2.0713</v>
       </c>
       <c r="O23" s="1">
         <v>0.63</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E24" s="1">
         <v>0.2</v>
@@ -1852,7 +2342,7 @@
         <v>32</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H24" s="1">
         <v>2000</v>
@@ -1861,39 +2351,39 @@
         <v>50</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L24" s="1">
-        <v>9.1499999999999998E-2</v>
+        <v>0.0915</v>
       </c>
       <c r="M24" s="1">
-        <v>0.96609999999999996</v>
+        <v>0.9661</v>
       </c>
       <c r="N24" s="1">
-        <v>1.2065999999999999</v>
+        <v>1.2066</v>
       </c>
       <c r="O24" s="1">
         <v>0.76</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E25" s="1">
         <v>0.2</v>
@@ -1902,7 +2392,7 @@
         <v>32</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H25" s="1">
         <v>2000</v>
@@ -1911,39 +2401,39 @@
         <v>20</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L25" s="1">
-        <v>0.13519999999999999</v>
+        <v>0.1352</v>
       </c>
       <c r="M25" s="1">
-        <v>0.95030000000000003</v>
+        <v>0.9503</v>
       </c>
       <c r="N25" s="1">
-        <v>0.62839999999999996</v>
+        <v>0.6284</v>
       </c>
       <c r="O25" s="1">
         <v>0.83</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E26" s="1">
         <v>0.2</v>
@@ -1952,7 +2442,7 @@
         <v>32</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H26" s="1">
         <v>2000</v>
@@ -1961,39 +2451,39 @@
         <v>50</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L26" s="1">
-        <v>6.4299999999999996E-2</v>
+        <v>0.0643</v>
       </c>
       <c r="M26" s="1">
-        <v>0.97670000000000001</v>
+        <v>0.9767</v>
       </c>
       <c r="N26" s="1">
-        <v>1.0512999999999999</v>
+        <v>1.0513</v>
       </c>
       <c r="O26" s="1">
         <v>0.77</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E27" s="1">
         <v>0.2</v>
@@ -2002,7 +2492,7 @@
         <v>32</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H27" s="1">
         <v>2000</v>
@@ -2011,39 +2501,39 @@
         <v>23</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L27" s="1">
-        <v>4.87E-2</v>
+        <v>0.0487</v>
       </c>
       <c r="M27" s="1">
-        <v>0.98319999999999996</v>
+        <v>0.9832</v>
       </c>
       <c r="N27" s="1">
-        <v>0.96050000000000002</v>
+        <v>0.9605</v>
       </c>
       <c r="O27" s="1">
         <v>0.83</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E28" s="1">
         <v>0.2</v>
@@ -2052,7 +2542,7 @@
         <v>32</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H28" s="1">
         <v>2000</v>
@@ -2061,16 +2551,16 @@
         <v>2</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L28" s="1">
-        <v>1.12E-2</v>
+        <v>0.0112</v>
       </c>
       <c r="M28" s="1">
-        <v>0.99639999999999995</v>
+        <v>0.9964</v>
       </c>
       <c r="N28" s="1">
         <v>2.0585</v>
@@ -2079,21 +2569,21 @@
         <v>0.71</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E29" s="1">
         <v>23000</v>
@@ -2102,7 +2592,7 @@
         <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H29" s="1">
         <v>2000</v>
@@ -2111,39 +2601,39 @@
         <v>2</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="L29" s="1">
-        <v>1.47E-2</v>
+        <v>0.0147</v>
       </c>
       <c r="M29" s="1">
-        <v>0.99550000000000005</v>
+        <v>0.9955</v>
       </c>
       <c r="N29" s="1">
-        <v>2.3279000000000001</v>
+        <v>2.3279</v>
       </c>
       <c r="O29" s="1">
-        <v>0.68530000000000002</v>
+        <v>0.6853</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E30" s="1">
         <v>23000</v>
@@ -2152,7 +2642,7 @@
         <v>32</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H30" s="1">
         <v>2000</v>
@@ -2161,39 +2651,39 @@
         <v>2</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L30" s="1">
-        <v>1.7100000000000001E-2</v>
+        <v>0.0171</v>
       </c>
       <c r="M30" s="1">
-        <v>0.99399999999999999</v>
+        <v>0.994</v>
       </c>
       <c r="N30" s="1">
-        <v>3.1293000000000002</v>
+        <v>3.1293</v>
       </c>
       <c r="O30" s="1">
         <v>0.66</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E31" s="1">
         <v>23000</v>
@@ -2202,7 +2692,7 @@
         <v>32</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H31" s="1">
         <v>2000</v>
@@ -2211,39 +2701,39 @@
         <v>5</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L31" s="1">
-        <v>3.1199999999999999E-2</v>
+        <v>0.0312</v>
       </c>
       <c r="M31" s="1">
-        <v>0.98850000000000005</v>
+        <v>0.9885</v>
       </c>
       <c r="N31" s="1">
-        <v>1.3498000000000001</v>
+        <v>1.3498</v>
       </c>
       <c r="O31" s="1">
-        <v>0.73780000000000001</v>
+        <v>0.7378</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="1" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E32" s="1">
         <v>23000</v>
@@ -2252,7 +2742,7 @@
         <v>32</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H32" s="1">
         <v>2000</v>
@@ -2261,39 +2751,39 @@
         <v>2</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L32" s="1">
-        <v>1.84E-2</v>
+        <v>0.0184</v>
       </c>
       <c r="M32" s="1">
-        <v>0.99399999999999999</v>
+        <v>0.994</v>
       </c>
       <c r="N32" s="1">
-        <v>2.0674000000000001</v>
+        <v>2.0674</v>
       </c>
       <c r="O32" s="1">
-        <v>0.63490000000000002</v>
+        <v>0.6349</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E33" s="1">
         <v>23000</v>
@@ -2302,7 +2792,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H33" s="1">
         <v>2000</v>
@@ -2311,39 +2801,39 @@
         <v>20</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L33" s="1">
-        <v>0.17330000000000001</v>
+        <v>0.1733</v>
       </c>
       <c r="M33" s="1">
-        <v>0.93279999999999996</v>
+        <v>0.9328</v>
       </c>
       <c r="N33" s="1">
-        <v>0.87029999999999996</v>
+        <v>0.8703</v>
       </c>
       <c r="O33" s="1">
         <v>0.8165</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E34" s="1">
         <v>23000</v>
@@ -2352,7 +2842,7 @@
         <v>32</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H34" s="1">
         <v>2000</v>
@@ -2361,10 +2851,10 @@
         <v>50</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L34" s="1">
         <v>0.1069</v>
@@ -2376,24 +2866,24 @@
         <v>1.0205</v>
       </c>
       <c r="O34" s="1">
-        <v>0.78549999999999998</v>
+        <v>0.7855</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E35" s="1">
         <v>23000</v>
@@ -2402,7 +2892,7 @@
         <v>32</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H35" s="1">
         <v>2000</v>
@@ -2411,39 +2901,39 @@
         <v>50</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L35" s="1">
-        <v>5.8400000000000001E-2</v>
+        <v>0.0584</v>
       </c>
       <c r="M35" s="1">
         <v>0.9788</v>
       </c>
       <c r="N35" s="1">
-        <v>0.98119999999999996</v>
+        <v>0.9812</v>
       </c>
       <c r="O35" s="1">
-        <v>0.79079999999999995</v>
+        <v>0.7908</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E36" s="1">
         <v>23000</v>
@@ -2452,7 +2942,7 @@
         <v>16</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H36" s="1">
         <v>2000</v>
@@ -2461,33 +2951,51 @@
         <v>50</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="L36" s="1">
-        <v>5.0099999999999999E-2</v>
+        <v>0.0501</v>
       </c>
       <c r="M36" s="1">
-        <v>0.98240000000000005</v>
+        <v>0.9824</v>
       </c>
       <c r="N36" s="1">
-        <v>0.48659999999999998</v>
+        <v>0.4866</v>
       </c>
       <c r="O36" s="1">
-        <v>0.88490000000000002</v>
+        <v>0.8849</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="Q36" t="s">
-        <v>78</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>